<commit_message>
Python and html fixed
</commit_message>
<xml_diff>
--- a/database/user.xlsx
+++ b/database/user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juelb\PycharmProjects\DynamicResumePython\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB3C667-81BD-46D6-A962-0E0689B070A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD38F70-0CAE-40D4-8BE0-C21CAF8A8423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="555" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="555" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDUCATION" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="196">
   <si>
     <t>TID</t>
   </si>
@@ -173,9 +173,6 @@
     <t>GIT</t>
   </si>
   <si>
-    <t>KAGGLE</t>
-  </si>
-  <si>
     <t>TB101</t>
   </si>
   <si>
@@ -191,15 +188,6 @@
     <t>juelbasak@gmail.com</t>
   </si>
   <si>
-    <t>linkedin.com/in/biswajit-basak-30bba185</t>
-  </si>
-  <si>
-    <t>github.com/thecuriousjuel</t>
-  </si>
-  <si>
-    <t>kaggle.com/juelbasak</t>
-  </si>
-  <si>
     <t>SKILL_NAME</t>
   </si>
   <si>
@@ -416,9 +404,6 @@
     <t>Income Prediction using XGBoost Algorithm</t>
   </si>
   <si>
-    <t>https://github.com/thecuriousjuel/ncome-Prediction</t>
-  </si>
-  <si>
     <t>https://income-prediction-xgboost.herokuapp.com/</t>
   </si>
   <si>
@@ -564,9 +549,6 @@
   </si>
   <si>
     <t>Design and development of an application for Election Analysis and Voting</t>
-  </si>
-  <si>
-    <t>https://github.com/thecuriousjuel/Mini-Project-BTech</t>
   </si>
   <si>
     <t>02/2018</t>
@@ -621,12 +603,36 @@
   <si>
     <t>2 Weeks</t>
   </si>
+  <si>
+    <t>https://github.com/thecuriousjuel/income-Prediction</t>
+  </si>
+  <si>
+    <t>https://github.com/thecuriousjuel/Mini-Project-Btech</t>
+  </si>
+  <si>
+    <t>linkedin.com/in/thecuriousjuel</t>
+  </si>
+  <si>
+    <t>github.com/thecuriousjuel</t>
+  </si>
+  <si>
+    <t>LEETCODE</t>
+  </si>
+  <si>
+    <t>leetcode.com/thecuriousjuel</t>
+  </si>
+  <si>
+    <t>YOUTUBE</t>
+  </si>
+  <si>
+    <t>youtube.com/@juelbasak</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,6 +651,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -654,7 +668,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -677,11 +691,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -689,8 +715,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1057,7 +1088,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1130,10 +1161,10 @@
         <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -1141,7 +1172,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -1156,10 +1187,10 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1250,13 +1281,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,36 +1322,46 @@
         <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
+      <c r="F2" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>193</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://www.linkedin.com/in/thecuriousjuel" xr:uid="{75845E7B-D671-48B6-8C32-1F9B902555E7}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{88BE6F1B-9D96-4C9B-B31A-5F887CCF6A83}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1328,87 +1381,87 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1429,39 +1482,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1474,7 +1527,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,16 +1544,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1517,115 +1570,115 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>98</v>
-      </c>
-      <c r="C3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" t="s">
-        <v>102</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" t="s">
         <v>110</v>
       </c>
-      <c r="B5" t="s">
+      <c r="G5" t="s">
         <v>111</v>
       </c>
-      <c r="C5" t="s">
+      <c r="I5" t="s">
         <v>112</v>
-      </c>
-      <c r="D5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I5" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1637,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,13 +1711,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -1679,21 +1732,21 @@
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" t="s">
-        <v>123</v>
+        <v>118</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -1702,297 +1755,310 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" t="s">
         <v>127</v>
       </c>
-      <c r="B3" t="s">
+      <c r="I3" t="s">
         <v>128</v>
-      </c>
-      <c r="C3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" t="s">
-        <v>193</v>
-      </c>
-      <c r="H3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" t="s">
-        <v>136</v>
+        <v>130</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" t="s">
+        <v>187</v>
+      </c>
+      <c r="H5" t="s">
         <v>139</v>
-      </c>
-      <c r="B5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G5" t="s">
-        <v>193</v>
-      </c>
-      <c r="H5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" t="s">
-        <v>147</v>
+        <v>141</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" t="s">
         <v>150</v>
-      </c>
-      <c r="B7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" t="s">
-        <v>154</v>
-      </c>
-      <c r="G7" t="s">
-        <v>193</v>
-      </c>
-      <c r="H7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" t="s">
-        <v>158</v>
+        <v>152</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G8" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C9" t="s">
-        <v>163</v>
+        <v>157</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="E9" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F9" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G9" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G10" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" t="s">
-        <v>173</v>
+        <v>167</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="E11" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I11" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" t="s">
+        <v>176</v>
+      </c>
+      <c r="I12" t="s">
         <v>177</v>
-      </c>
-      <c r="B12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" t="s">
-        <v>179</v>
-      </c>
-      <c r="E12" t="s">
-        <v>180</v>
-      </c>
-      <c r="F12" t="s">
-        <v>181</v>
-      </c>
-      <c r="G12" t="s">
-        <v>193</v>
-      </c>
-      <c r="H12" t="s">
-        <v>182</v>
-      </c>
-      <c r="I12" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G13" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H13" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{27932C6F-40E2-4785-88E4-2D167B687CA1}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{28A98B2A-223C-4E48-A83C-8E2D378476F0}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{C53B80C8-AF6D-496B-8BFC-5FC618DCCA4B}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{7956B274-B42D-4CED-8C28-67AAAF7485CE}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{D99139F7-287C-4E09-8136-9796A36EFFAB}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00A8B42C-94BC-4EAB-82B9-2ED6426DEE17}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{EA07B4E0-3E3A-4C48-A74F-A606517FDFD2}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{6A942992-D241-45BE-AE7F-48DBCA5084EA}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{91B1D9BA-4053-4982-934D-2D091A77DB2C}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{96917340-78F0-483C-9643-17147667F4A8}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{D94DEDC6-BCD4-43A6-A78E-C5F7564E3593}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>